<commit_message>
Update to IPTp and bednet effect on SGA birth outcome
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="28160" windowHeight="14280" tabRatio="500" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="3140" yWindow="-20620" windowWidth="26140" windowHeight="17680" tabRatio="500" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -2677,6 +2677,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
     <comment ref="C3" authorId="0">
@@ -2700,6 +2701,102 @@
           </rPr>
           <t xml:space="preserve">
 Poor pregnant women - all target population</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -3305,7 +3402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="184">
   <si>
     <t>year</t>
   </si>
@@ -6604,8 +6701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8045,10 +8142,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8187,6 +8284,84 @@
       </c>
       <c r="F7" s="10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="47">
+        <v>0.35</v>
+      </c>
+      <c r="D8" s="47">
+        <v>0.35</v>
+      </c>
+      <c r="E8" s="47">
+        <v>0</v>
+      </c>
+      <c r="F8" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9">
+        <f>'Baseline year demographics'!C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="D9">
+        <f>'Baseline year demographics'!C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="47">
+        <v>0</v>
+      </c>
+      <c r="F9" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="47">
+        <v>0.35</v>
+      </c>
+      <c r="D10" s="47">
+        <v>0.35</v>
+      </c>
+      <c r="E10" s="47">
+        <v>0</v>
+      </c>
+      <c r="F10" s="47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11">
+        <f>'Baseline year demographics'!C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <f>'Baseline year demographics'!C8</f>
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="47">
+        <v>0</v>
+      </c>
+      <c r="F11" s="47">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -9663,7 +9838,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9951,8 +10126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Updated spreadsheet with wasting data
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14280" tabRatio="500" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -884,8 +884,53 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Sam</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
+    <comment ref="F18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Should be targetting the frac poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO statement</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D24" authorId="0">
       <text>
         <r>
@@ -1362,6 +1407,50 @@
         </r>
       </text>
     </comment>
+    <comment ref="D39" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Per person per year</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D40" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Made up, a bit less per treatment than PPCF per year</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -3227,7 +3316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="193">
   <si>
     <t>year</t>
   </si>
@@ -3760,18 +3849,6 @@
     <t>Zinc supplementation</t>
   </si>
   <si>
-    <t>Wasting (moderate)</t>
-  </si>
-  <si>
-    <t>Wasting (high)</t>
-  </si>
-  <si>
-    <t>OR wasting (high)</t>
-  </si>
-  <si>
-    <t>OR wasting (moderate)</t>
-  </si>
-  <si>
     <t>saturation coverage</t>
   </si>
   <si>
@@ -3781,24 +3858,6 @@
     <t>Cash transfers</t>
   </si>
   <si>
-    <t>Treatment of wasting (moderate)</t>
-  </si>
-  <si>
-    <t>Treatment of wasting (high)</t>
-  </si>
-  <si>
-    <t>OR severe wasting by intervention</t>
-  </si>
-  <si>
-    <t>OR moderate wasting by intervention</t>
-  </si>
-  <si>
-    <t>OR severe wasting by condition</t>
-  </si>
-  <si>
-    <t>OR moderate wasting by condition</t>
-  </si>
-  <si>
     <t>IFA fortification of wheat flour</t>
   </si>
   <si>
@@ -3806,6 +3865,36 @@
   </si>
   <si>
     <t>IFA fortification of rice</t>
+  </si>
+  <si>
+    <t>MAM</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>OR SAM</t>
+  </si>
+  <si>
+    <t>OR MAM</t>
+  </si>
+  <si>
+    <t>OR SAM by condition</t>
+  </si>
+  <si>
+    <t>OR MAM by condition</t>
+  </si>
+  <si>
+    <t>Treatment of MAM</t>
+  </si>
+  <si>
+    <t>Treatment of SAM</t>
+  </si>
+  <si>
+    <t>OR SAM by intervention</t>
+  </si>
+  <si>
+    <t>OR MAM by intervention</t>
   </si>
 </sst>
 </file>
@@ -3814,11 +3903,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -4593,16 +4682,16 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -4621,10 +4710,10 @@
     <xf numFmtId="10" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -4633,12 +4722,12 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6580,7 +6669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -6923,8 +7012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7221,10 +7310,10 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C11" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="70">
         <v>1</v>
@@ -7247,10 +7336,10 @@
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C12" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" s="70">
         <v>1</v>
@@ -7273,10 +7362,10 @@
     </row>
     <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C13" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="70">
         <v>1</v>
@@ -7990,7 +8079,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
@@ -8021,7 +8110,7 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="12" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
@@ -8052,7 +8141,7 @@
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
@@ -9635,7 +9724,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B31" s="61" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -9679,7 +9768,7 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B32" s="61" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -9723,7 +9812,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B33" s="61" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -9792,7 +9881,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9826,48 +9915,48 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C2" s="60">
         <v>1</v>
       </c>
       <c r="D2" s="60">
-        <v>0.9</v>
+        <v>0.21</v>
       </c>
       <c r="E2" s="60">
-        <v>0.9</v>
+        <v>0.21</v>
       </c>
       <c r="F2" s="60">
-        <v>0.6</v>
+        <v>0.21</v>
       </c>
       <c r="G2" s="60">
-        <v>0.6</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B4" s="61" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C4" s="60">
         <v>1</v>
       </c>
       <c r="D4" s="60">
-        <v>0.9</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E4" s="60">
-        <v>0.9</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="F4" s="60">
-        <v>0.6</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="G4" s="60">
-        <v>0.6</v>
+        <v>0.14299999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -9884,7 +9973,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10021,7 +10110,7 @@
         <v>161</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>124</v>
@@ -10084,7 +10173,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>124</v>
@@ -10150,7 +10239,7 @@
         <v>84</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>124</v>
@@ -10213,7 +10302,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>124</v>
@@ -10276,10 +10365,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>124</v>
@@ -10331,7 +10420,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="61">
-        <v>0.62</v>
+        <v>0.7</v>
       </c>
       <c r="G20" s="61">
         <v>0.62</v>
@@ -10342,7 +10431,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>124</v>
@@ -10394,7 +10483,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="68">
-        <v>0.62</v>
+        <v>0.84</v>
       </c>
       <c r="G23" s="68">
         <v>0.62</v>
@@ -10405,7 +10494,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
@@ -10453,7 +10542,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
@@ -10502,7 +10591,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B28" t="s">
         <v>45</v>
@@ -10559,8 +10648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10579,10 +10668,10 @@
         <v>123</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -11049,7 +11138,7 @@
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="12" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B35" s="19">
         <v>0</v>
@@ -11063,7 +11152,7 @@
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="12" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B36" s="19">
         <v>0</v>
@@ -11077,7 +11166,7 @@
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="12" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B37" s="19">
         <v>0</v>
@@ -11105,7 +11194,7 @@
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B39" s="14">
         <v>0</v>
@@ -11114,12 +11203,13 @@
         <v>0.85</v>
       </c>
       <c r="D39" s="19">
-        <v>1</v>
+        <f>180/12</f>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B40" s="14">
         <v>0</v>
@@ -11128,21 +11218,23 @@
         <v>0.85</v>
       </c>
       <c r="D40" s="19">
-        <v>1</v>
+        <f>30*(52/8)</f>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="B41" s="14">
-        <v>0</v>
+        <v>0.61</v>
       </c>
       <c r="C41" s="13">
         <v>0.85</v>
       </c>
       <c r="D41" s="19">
-        <v>1</v>
+        <f>179.97*(52/8)</f>
+        <v>1169.8050000000001</v>
       </c>
     </row>
   </sheetData>
@@ -12450,7 +12542,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -12537,7 +12629,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B5" s="60">
         <f>Distributions!C10/100 * 1.6</f>
@@ -12562,7 +12654,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="B6" s="60">
         <f>Distributions!C11/100 * 1.6</f>
@@ -12919,7 +13011,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13078,7 +13170,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="C10" s="17">
         <v>15</v>
@@ -13098,7 +13190,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="C11" s="17">
         <v>4.9000000000000004</v>
@@ -13212,7 +13304,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13295,7 +13387,7 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C5" s="67">
         <v>1</v>
@@ -13312,7 +13404,7 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="C6" s="67">
         <v>1</v>
@@ -13496,8 +13588,8 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14069,7 +14161,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C26" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -14092,7 +14184,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C27" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D27" s="4">
         <v>1</v>
@@ -14164,7 +14256,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C30" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -14187,7 +14279,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C31" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
@@ -14259,7 +14351,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C34" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
@@ -14282,7 +14374,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C35" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D35" s="4">
         <v>1</v>
@@ -14354,7 +14446,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C38" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
@@ -14377,7 +14469,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C39" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -14449,7 +14541,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C42" s="4" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -14472,7 +14564,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C43" s="4" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -15423,10 +15515,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15672,7 +15764,7 @@
     <row r="14" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>28</v>
@@ -15695,7 +15787,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
@@ -15714,6 +15806,220 @@
       </c>
       <c r="G17" s="60">
         <v>1.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="61">
+        <v>1</v>
+      </c>
+      <c r="D19" s="61">
+        <v>1</v>
+      </c>
+      <c r="E19" s="61">
+        <v>1</v>
+      </c>
+      <c r="F19" s="61">
+        <v>1</v>
+      </c>
+      <c r="G19" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="61">
+        <v>1</v>
+      </c>
+      <c r="D20" s="61">
+        <v>1</v>
+      </c>
+      <c r="E20" s="61">
+        <v>1</v>
+      </c>
+      <c r="F20" s="61">
+        <v>1</v>
+      </c>
+      <c r="G20" s="61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="61">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="E21" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="F21" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="G21" s="61">
+        <v>1.498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B22" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="61">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="E22" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="F22" s="61">
+        <v>1.498</v>
+      </c>
+      <c r="G22" s="61">
+        <v>1.498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="61">
+        <v>1.64</v>
+      </c>
+      <c r="D23" s="61">
+        <v>1.641</v>
+      </c>
+      <c r="E23" s="61">
+        <v>1.641</v>
+      </c>
+      <c r="F23" s="61">
+        <v>1.641</v>
+      </c>
+      <c r="G23" s="61">
+        <v>1.641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B24" s="4"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="68">
+        <v>1</v>
+      </c>
+      <c r="D25" s="68">
+        <v>1</v>
+      </c>
+      <c r="E25" s="68">
+        <v>1</v>
+      </c>
+      <c r="F25" s="68">
+        <v>1</v>
+      </c>
+      <c r="G25" s="68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="68">
+        <v>1</v>
+      </c>
+      <c r="D26" s="68">
+        <v>1</v>
+      </c>
+      <c r="E26" s="68">
+        <v>1</v>
+      </c>
+      <c r="F26" s="68">
+        <v>1</v>
+      </c>
+      <c r="G26" s="68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B27" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="E27" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="F27" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="G27" s="68">
+        <v>1.498</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B28" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C28" s="68">
+        <v>1.5</v>
+      </c>
+      <c r="D28" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="E28" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="F28" s="68">
+        <v>1.498</v>
+      </c>
+      <c r="G28" s="68">
+        <v>1.498</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="68">
+        <v>1.64</v>
+      </c>
+      <c r="D29" s="68">
+        <v>1.641</v>
+      </c>
+      <c r="E29" s="68">
+        <v>1.641</v>
+      </c>
+      <c r="F29" s="68">
+        <v>1.641</v>
+      </c>
+      <c r="G29" s="68">
+        <v>1.641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated birth outcome OR for wasting
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="-20960" windowWidth="28940" windowHeight="20960" tabRatio="500" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -855,7 +855,7 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="F14" authorId="0">
+    <comment ref="F18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -877,7 +877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="1">
+    <comment ref="F21" authorId="1">
       <text>
         <r>
           <rPr>
@@ -899,7 +899,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0">
+    <comment ref="D22" authorId="0">
       <text>
         <r>
           <rPr>
@@ -921,7 +921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0">
+    <comment ref="D23" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3306,7 +3306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="193">
   <si>
     <t>year</t>
   </si>
@@ -4733,9 +4733,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -4746,6 +4743,9 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="547">
@@ -7302,19 +7302,19 @@
       <c r="B11" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="70">
-        <v>0</v>
-      </c>
-      <c r="D11" s="70">
-        <v>1</v>
-      </c>
-      <c r="E11" s="70">
-        <v>1</v>
-      </c>
-      <c r="F11" s="70">
-        <v>1</v>
-      </c>
-      <c r="G11" s="70">
+      <c r="C11" s="69">
+        <v>0</v>
+      </c>
+      <c r="D11" s="69">
+        <v>1</v>
+      </c>
+      <c r="E11" s="69">
+        <v>1</v>
+      </c>
+      <c r="F11" s="69">
+        <v>1</v>
+      </c>
+      <c r="G11" s="69">
         <v>1</v>
       </c>
       <c r="H11" s="3">
@@ -7328,19 +7328,19 @@
       <c r="B12" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="70">
-        <v>0</v>
-      </c>
-      <c r="D12" s="70">
-        <v>1</v>
-      </c>
-      <c r="E12" s="70">
-        <v>1</v>
-      </c>
-      <c r="F12" s="70">
-        <v>1</v>
-      </c>
-      <c r="G12" s="70">
+      <c r="C12" s="69">
+        <v>0</v>
+      </c>
+      <c r="D12" s="69">
+        <v>1</v>
+      </c>
+      <c r="E12" s="69">
+        <v>1</v>
+      </c>
+      <c r="F12" s="69">
+        <v>1</v>
+      </c>
+      <c r="G12" s="69">
         <v>1</v>
       </c>
       <c r="H12" s="3">
@@ -7354,19 +7354,19 @@
       <c r="B13" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="70">
-        <v>0</v>
-      </c>
-      <c r="D13" s="70">
-        <v>1</v>
-      </c>
-      <c r="E13" s="70">
-        <v>1</v>
-      </c>
-      <c r="F13" s="70">
-        <v>1</v>
-      </c>
-      <c r="G13" s="70">
+      <c r="C13" s="69">
+        <v>0</v>
+      </c>
+      <c r="D13" s="69">
+        <v>1</v>
+      </c>
+      <c r="E13" s="69">
+        <v>1</v>
+      </c>
+      <c r="F13" s="69">
+        <v>1</v>
+      </c>
+      <c r="G13" s="69">
         <v>1</v>
       </c>
       <c r="H13" s="3">
@@ -8077,23 +8077,23 @@
       <c r="D42" s="3">
         <v>0</v>
       </c>
-      <c r="E42" s="72">
+      <c r="E42" s="71">
         <f>'[1]Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="F42" s="72">
+      <c r="F42" s="71">
         <f>'[1]Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="G42" s="72">
+      <c r="G42" s="71">
         <f>'[1]Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="H42" s="72">
+      <c r="H42" s="71">
         <f>'[1]Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
-      <c r="I42" s="72">
+      <c r="I42" s="71">
         <f>'[1]Baseline year demographics'!$C$21</f>
         <v>0.12</v>
       </c>
@@ -8108,23 +8108,23 @@
       <c r="D43" s="3">
         <v>0</v>
       </c>
-      <c r="E43" s="70">
+      <c r="E43" s="69">
         <f>'[1]Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="F43" s="70">
+      <c r="F43" s="69">
         <f>'[1]Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="G43" s="70">
+      <c r="G43" s="69">
         <f>'[1]Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="H43" s="70">
+      <c r="H43" s="69">
         <f>'[1]Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
-      <c r="I43" s="70">
+      <c r="I43" s="69">
         <f>'[1]Baseline year demographics'!$C$22</f>
         <v>0.05</v>
       </c>
@@ -8139,23 +8139,23 @@
       <c r="D44" s="3">
         <v>0</v>
       </c>
-      <c r="E44" s="70">
+      <c r="E44" s="69">
         <f>'[1]Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="F44" s="70">
+      <c r="F44" s="69">
         <f>'[1]Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="G44" s="70">
+      <c r="G44" s="69">
         <f>'[1]Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="H44" s="70">
+      <c r="H44" s="69">
         <f>'[1]Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
-      <c r="I44" s="70">
+      <c r="I44" s="69">
         <f>'[1]Baseline year demographics'!$C$20</f>
         <v>0.8</v>
       </c>
@@ -9959,10 +9959,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10273,10 +10273,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>179</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="A14" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>184</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -10309,7 +10309,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="61">
-        <v>0.7</v>
+        <v>0.62</v>
       </c>
       <c r="G15" s="61">
         <v>0.62</v>
@@ -10325,19 +10325,19 @@
       <c r="C16" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="68">
-        <v>0</v>
-      </c>
-      <c r="E16" s="68">
-        <v>0</v>
-      </c>
-      <c r="F16" s="68">
+      <c r="D16" s="61">
+        <v>0</v>
+      </c>
+      <c r="E16" s="61">
+        <v>0</v>
+      </c>
+      <c r="F16" s="61">
         <v>0.33500000000000002</v>
       </c>
-      <c r="G16" s="69">
+      <c r="G16" s="62">
         <v>0.33500000000000002</v>
       </c>
-      <c r="H16" s="69">
+      <c r="H16" s="62">
         <v>0.33500000000000002</v>
       </c>
     </row>
@@ -10345,122 +10345,117 @@
       <c r="C17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="68">
-        <v>0</v>
-      </c>
-      <c r="E17" s="68">
-        <v>0</v>
-      </c>
-      <c r="F17" s="68">
-        <v>0.84</v>
-      </c>
-      <c r="G17" s="68">
+      <c r="D17" s="61">
+        <v>0</v>
+      </c>
+      <c r="E17" s="61">
+        <v>0</v>
+      </c>
+      <c r="F17" s="61">
         <v>0.62</v>
       </c>
-      <c r="H17" s="68">
+      <c r="G17" s="61">
         <v>0.62</v>
       </c>
+      <c r="H17" s="61">
+        <v>0.62</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A18" s="12" t="s">
-        <v>180</v>
+      <c r="A18" t="s">
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="61">
+        <v>0</v>
+      </c>
+      <c r="E18" s="61">
+        <v>0</v>
+      </c>
+      <c r="F18" s="61">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G18" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H18" s="62">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="61">
+        <v>0</v>
+      </c>
+      <c r="E19" s="61">
+        <v>0</v>
+      </c>
+      <c r="F19" s="61">
         <v>0.7</v>
       </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12">
-        <v>0</v>
-      </c>
-      <c r="G18" s="12">
-        <v>0</v>
-      </c>
-      <c r="H18" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A19" s="12"/>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0</v>
-      </c>
-      <c r="F19" s="12">
-        <v>0</v>
-      </c>
-      <c r="G19" s="12">
-        <v>0</v>
-      </c>
-      <c r="H19" s="12">
-        <v>0</v>
+      <c r="G19" s="61">
+        <v>0.62</v>
+      </c>
+      <c r="H19" s="61">
+        <v>0.62</v>
       </c>
       <c r="I19" s="11"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A20" s="12" t="s">
-        <v>181</v>
-      </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="12">
-        <v>0.7</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <v>0</v>
+      <c r="D20" s="67">
+        <v>0</v>
+      </c>
+      <c r="E20" s="67">
+        <v>0</v>
+      </c>
+      <c r="F20" s="67">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G20" s="68">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="H20" s="68">
+        <v>0.33500000000000002</v>
       </c>
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A21" s="12"/>
-      <c r="C21" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.46</v>
-      </c>
-      <c r="E21" s="12">
-        <v>0</v>
-      </c>
-      <c r="F21" s="12">
-        <v>0</v>
-      </c>
-      <c r="G21" s="12">
-        <v>0</v>
-      </c>
-      <c r="H21" s="12">
-        <v>0</v>
+      <c r="C21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="67">
+        <v>0</v>
+      </c>
+      <c r="E21" s="67">
+        <v>0</v>
+      </c>
+      <c r="F21" s="67">
+        <v>0.84</v>
+      </c>
+      <c r="G21" s="67">
+        <v>0.62</v>
+      </c>
+      <c r="H21" s="67">
+        <v>0.62</v>
       </c>
       <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B22" t="s">
         <v>45</v>
@@ -10486,6 +10481,7 @@
       <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="12"/>
       <c r="C23" t="s">
         <v>68</v>
       </c>
@@ -10505,6 +10501,99 @@
         <v>0</v>
       </c>
       <c r="I23" s="11"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A24" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E24" s="12">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>0</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A25" s="12"/>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="E25" s="12">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A26" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="12">
+        <v>0.7</v>
+      </c>
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="12">
+        <v>0.46</v>
+      </c>
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
+        <v>0</v>
+      </c>
+      <c r="H27" s="12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10517,8 +10606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -10623,7 +10712,7 @@
       <c r="C7" s="64">
         <v>0.85</v>
       </c>
-      <c r="D7" s="71">
+      <c r="D7" s="70">
         <v>50</v>
       </c>
     </row>
@@ -10651,7 +10740,7 @@
       <c r="C9" s="64">
         <v>0.85</v>
       </c>
-      <c r="D9" s="71">
+      <c r="D9" s="70">
         <v>1</v>
       </c>
     </row>
@@ -11072,8 +11161,8 @@
         <v>0.85</v>
       </c>
       <c r="D39" s="19">
-        <f>180/12</f>
-        <v>15</v>
+        <f>180</f>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13173,7 +13262,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13258,34 +13347,34 @@
       <c r="B5" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="67">
-        <v>1</v>
-      </c>
-      <c r="D5" s="67">
-        <v>1</v>
-      </c>
-      <c r="E5" s="67">
-        <v>1</v>
-      </c>
-      <c r="F5" s="67">
-        <v>1</v>
+      <c r="C5" s="72">
+        <v>1</v>
+      </c>
+      <c r="D5" s="72">
+        <v>2.58</v>
+      </c>
+      <c r="E5" s="72">
+        <v>1.65</v>
+      </c>
+      <c r="F5" s="72">
+        <v>3.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>185</v>
       </c>
-      <c r="C6" s="67">
-        <v>1</v>
-      </c>
-      <c r="D6" s="67">
-        <v>1</v>
-      </c>
-      <c r="E6" s="67">
-        <v>1</v>
-      </c>
-      <c r="F6" s="67">
-        <v>1</v>
+      <c r="C6" s="72">
+        <v>1</v>
+      </c>
+      <c r="D6" s="72">
+        <v>2.58</v>
+      </c>
+      <c r="E6" s="72">
+        <v>1.65</v>
+      </c>
+      <c r="F6" s="72">
+        <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15795,19 +15884,19 @@
       <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="68">
-        <v>1</v>
-      </c>
-      <c r="D25" s="68">
-        <v>1</v>
-      </c>
-      <c r="E25" s="68">
-        <v>1</v>
-      </c>
-      <c r="F25" s="68">
-        <v>1</v>
-      </c>
-      <c r="G25" s="68">
+      <c r="C25" s="67">
+        <v>1</v>
+      </c>
+      <c r="D25" s="67">
+        <v>1</v>
+      </c>
+      <c r="E25" s="67">
+        <v>1</v>
+      </c>
+      <c r="F25" s="67">
+        <v>1</v>
+      </c>
+      <c r="G25" s="67">
         <v>1</v>
       </c>
     </row>
@@ -15815,19 +15904,19 @@
       <c r="B26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="68">
-        <v>1</v>
-      </c>
-      <c r="D26" s="68">
-        <v>1</v>
-      </c>
-      <c r="E26" s="68">
-        <v>1</v>
-      </c>
-      <c r="F26" s="68">
-        <v>1</v>
-      </c>
-      <c r="G26" s="68">
+      <c r="C26" s="67">
+        <v>1</v>
+      </c>
+      <c r="D26" s="67">
+        <v>1</v>
+      </c>
+      <c r="E26" s="67">
+        <v>1</v>
+      </c>
+      <c r="F26" s="67">
+        <v>1</v>
+      </c>
+      <c r="G26" s="67">
         <v>1</v>
       </c>
     </row>
@@ -15835,19 +15924,19 @@
       <c r="B27" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="68">
+      <c r="C27" s="67">
         <v>1.5</v>
       </c>
-      <c r="D27" s="68">
+      <c r="D27" s="67">
         <v>1.498</v>
       </c>
-      <c r="E27" s="68">
+      <c r="E27" s="67">
         <v>1.498</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="67">
         <v>1.498</v>
       </c>
-      <c r="G27" s="68">
+      <c r="G27" s="67">
         <v>1.498</v>
       </c>
     </row>
@@ -15855,19 +15944,19 @@
       <c r="B28" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="68">
+      <c r="C28" s="67">
         <v>1.5</v>
       </c>
-      <c r="D28" s="68">
+      <c r="D28" s="67">
         <v>1.498</v>
       </c>
-      <c r="E28" s="68">
+      <c r="E28" s="67">
         <v>1.498</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="67">
         <v>1.498</v>
       </c>
-      <c r="G28" s="68">
+      <c r="G28" s="67">
         <v>1.498</v>
       </c>
     </row>
@@ -15875,19 +15964,19 @@
       <c r="B29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="68">
+      <c r="C29" s="67">
         <v>1.64</v>
       </c>
-      <c r="D29" s="68">
+      <c r="D29" s="67">
         <v>1.641</v>
       </c>
-      <c r="E29" s="68">
+      <c r="E29" s="67">
         <v>1.641</v>
       </c>
-      <c r="F29" s="68">
+      <c r="F29" s="67">
         <v>1.641</v>
       </c>
-      <c r="G29" s="68">
+      <c r="G29" s="67">
         <v>1.641</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed unused data for wasting
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3259,7 +3259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="193">
   <si>
     <t>year</t>
   </si>
@@ -9852,7 +9852,7 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -15364,10 +15364,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -15657,220 +15657,6 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="61">
-        <v>1</v>
-      </c>
-      <c r="D19" s="61">
-        <v>1</v>
-      </c>
-      <c r="E19" s="61">
-        <v>1</v>
-      </c>
-      <c r="F19" s="61">
-        <v>1</v>
-      </c>
-      <c r="G19" s="61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="61">
-        <v>1</v>
-      </c>
-      <c r="D20" s="61">
-        <v>1</v>
-      </c>
-      <c r="E20" s="61">
-        <v>1</v>
-      </c>
-      <c r="F20" s="61">
-        <v>1</v>
-      </c>
-      <c r="G20" s="61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B21" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="D21" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="E21" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="F21" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="G21" s="61">
-        <v>1.498</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B22" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C22" s="61">
-        <v>1.5</v>
-      </c>
-      <c r="D22" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="E22" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="F22" s="61">
-        <v>1.498</v>
-      </c>
-      <c r="G22" s="61">
-        <v>1.498</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B23" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="61">
-        <v>1.64</v>
-      </c>
-      <c r="D23" s="61">
-        <v>1.641</v>
-      </c>
-      <c r="E23" s="61">
-        <v>1.641</v>
-      </c>
-      <c r="F23" s="61">
-        <v>1.641</v>
-      </c>
-      <c r="G23" s="61">
-        <v>1.641</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B24" s="4"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="67">
-        <v>1</v>
-      </c>
-      <c r="D25" s="67">
-        <v>1</v>
-      </c>
-      <c r="E25" s="67">
-        <v>1</v>
-      </c>
-      <c r="F25" s="67">
-        <v>1</v>
-      </c>
-      <c r="G25" s="67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B26" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="67">
-        <v>1</v>
-      </c>
-      <c r="D26" s="67">
-        <v>1</v>
-      </c>
-      <c r="E26" s="67">
-        <v>1</v>
-      </c>
-      <c r="F26" s="67">
-        <v>1</v>
-      </c>
-      <c r="G26" s="67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B27" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="67">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="E27" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="F27" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="G27" s="67">
-        <v>1.498</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B28" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="67">
-        <v>1.5</v>
-      </c>
-      <c r="D28" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="E28" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="F28" s="67">
-        <v>1.498</v>
-      </c>
-      <c r="G28" s="67">
-        <v>1.498</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B29" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="67">
-        <v>1.64</v>
-      </c>
-      <c r="D29" s="67">
-        <v>1.641</v>
-      </c>
-      <c r="E29" s="67">
-        <v>1.641</v>
-      </c>
-      <c r="F29" s="67">
-        <v>1.641</v>
-      </c>
-      <c r="G29" s="67">
-        <v>1.641</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
IYCF package data in spreadsheet
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,15 @@
     <sheet name="Birth outcomes &amp; risks" sheetId="6" r:id="rId7"/>
     <sheet name="Relative risks" sheetId="26" r:id="rId8"/>
     <sheet name="Odds ratios" sheetId="27" r:id="rId9"/>
-    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId10"/>
-    <sheet name="Interventions target population" sheetId="21" r:id="rId11"/>
-    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId12"/>
-    <sheet name="Interventions anemia" sheetId="30" r:id="rId13"/>
-    <sheet name="Interventions wasting" sheetId="31" r:id="rId14"/>
-    <sheet name="Interventions for children" sheetId="28" r:id="rId15"/>
-    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId16"/>
+    <sheet name="IYCF package odds ratios" sheetId="32" r:id="rId10"/>
+    <sheet name="IYCF packages" sheetId="33" r:id="rId11"/>
+    <sheet name="Appropriate breastfeeding" sheetId="19" r:id="rId12"/>
+    <sheet name="Interventions target population" sheetId="21" r:id="rId13"/>
+    <sheet name="Interventions birth outcomes" sheetId="22" r:id="rId14"/>
+    <sheet name="Interventions anemia" sheetId="30" r:id="rId15"/>
+    <sheet name="Interventions wasting" sheetId="31" r:id="rId16"/>
+    <sheet name="Interventions for children" sheetId="28" r:id="rId17"/>
+    <sheet name="Interventions cost and coverage" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -299,10 +301,9 @@
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -320,11 +321,11 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+Poor pregnant women - all target population</t>
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="1">
+    <comment ref="C9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -333,9 +334,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -344,11 +343,11 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="1">
+    <comment ref="D9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -357,9 +356,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -368,11 +365,11 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="1">
+    <comment ref="C11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -381,9 +378,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -392,11 +387,11 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="1">
+    <comment ref="D11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -405,9 +400,7 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -416,428 +409,7 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Source: WHO guidelines on sprinkles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Effect on iron-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Only in malaria risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-made this number up
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-Same effect as iron fortification</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -848,11 +420,34 @@
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Sam</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="F21" authorId="0">
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -861,7 +456,9 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -870,11 +467,11 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-WHO statement</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="1">
+    <comment ref="M2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -883,7 +480,9 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -892,11 +491,11 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="1">
+    <comment ref="N2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -905,7 +504,9 @@
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -914,7 +515,452 @@
             <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Source: WHO guidelines on sprinkles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Effect on iron-deficiency anemia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Only in malaria risk</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+made this number up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+Same effect as iron fortification</t>
         </r>
       </text>
     </comment>
@@ -923,6 +969,83 @@
 </file>
 
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="F21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO statement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -2026,1110 +2149,72 @@
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Janka Petravic</author>
-    <author>Ruth</author>
-    <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-food insecure - default poor</t>
+May not need this listed</t>
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="1">
+    <comment ref="A15" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-poor, not in malaria area
-</t>
+We currently do not have 'appropriate complementary feeding' data to use</t>
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="1">
+    <comment ref="B25" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
-poor, in malaria area
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, not in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Coverage of these interventions is mutually exclusive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I22" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I29" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
+May not need this group</t>
         </r>
       </text>
     </comment>
@@ -3140,11 +2225,12 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Janka Petravic</author>
+    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
-    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -3153,7 +2239,7 @@
             <color indexed="81"/>
             <rFont val="Arial"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -3162,95 +2248,1087 @@
             <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-Poor pregnant women - all target population</t>
+food insecure - default poor</t>
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="1">
+    <comment ref="E7" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, not in malaria area
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="1">
+    <comment ref="E8" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, in malaria area
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="1">
+    <comment ref="E9" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, not in malaria area</t>
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="1">
+    <comment ref="E10" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, in malaria area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Coverage of these interventions is mutually exclusive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I29" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -3259,7 +3337,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -3838,6 +3916,45 @@
   </si>
   <si>
     <t>OR MAM by intervention</t>
+  </si>
+  <si>
+    <t>Health facility</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Delivery mode</t>
+  </si>
+  <si>
+    <t>Behaviour</t>
+  </si>
+  <si>
+    <t>OR for correct breastfeeding</t>
+  </si>
+  <si>
+    <t>OR for correct complementary feeding</t>
+  </si>
+  <si>
+    <t>Target population</t>
+  </si>
+  <si>
+    <t>IYCF package</t>
+  </si>
+  <si>
+    <t>IYCF 1</t>
+  </si>
+  <si>
+    <t>IYCF 2</t>
+  </si>
+  <si>
+    <t>IYCF 3</t>
+  </si>
+  <si>
+    <t>Mass media</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -3952,7 +4069,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3995,6 +4112,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -4033,7 +4156,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="547">
+  <cellStyleXfs count="551">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4581,8 +4704,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4700,8 +4827,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="547">
+  <cellStyles count="551">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -4975,6 +5112,8 @@
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5247,6 +5386,8 @@
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="10" builtinId="5"/>
   </cellStyles>
@@ -6821,6 +6962,750 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="74">
+        <v>1.85</v>
+      </c>
+      <c r="E2" s="74">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G2" s="74">
+        <v>1.01</v>
+      </c>
+      <c r="H2" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B3" s="73"/>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="74">
+        <v>1.9</v>
+      </c>
+      <c r="E3" s="74">
+        <v>1.25</v>
+      </c>
+      <c r="F3" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G3" s="74">
+        <v>1.01</v>
+      </c>
+      <c r="H3" s="76">
+        <v>1</v>
+      </c>
+      <c r="J3" s="74"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B4" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" s="74">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="E4" s="74">
+        <v>3.07</v>
+      </c>
+      <c r="F4" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G4" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H4" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B5" s="73"/>
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="74">
+        <v>2.17</v>
+      </c>
+      <c r="E5" s="74">
+        <v>2.48</v>
+      </c>
+      <c r="F5" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G5" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H5" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B6" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+      <c r="D6" s="74">
+        <v>1</v>
+      </c>
+      <c r="E6" s="74">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="74">
+        <v>1.3</v>
+      </c>
+      <c r="G6" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H6" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B7" s="73"/>
+      <c r="C7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="74">
+        <v>1</v>
+      </c>
+      <c r="E7" s="74">
+        <v>1.5</v>
+      </c>
+      <c r="F7" s="74">
+        <v>1.25</v>
+      </c>
+      <c r="G7" s="74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B8" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="74">
+        <v>1</v>
+      </c>
+      <c r="E8" s="74">
+        <v>1</v>
+      </c>
+      <c r="F8" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G8" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H8" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B9" s="73"/>
+      <c r="C9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="74">
+        <v>1</v>
+      </c>
+      <c r="E9" s="74">
+        <v>1</v>
+      </c>
+      <c r="F9" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="G9" s="74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H9" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B10" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="74">
+        <v>1</v>
+      </c>
+      <c r="E10" s="74">
+        <v>1</v>
+      </c>
+      <c r="F10" s="74">
+        <v>1</v>
+      </c>
+      <c r="G10" s="74">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H10" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B11" s="73"/>
+      <c r="C11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" s="74">
+        <v>1</v>
+      </c>
+      <c r="E11" s="74">
+        <v>1</v>
+      </c>
+      <c r="F11" s="74">
+        <v>1</v>
+      </c>
+      <c r="G11" s="74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H11" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="74">
+        <v>1</v>
+      </c>
+      <c r="E12" s="74">
+        <v>1</v>
+      </c>
+      <c r="F12" s="74">
+        <v>1</v>
+      </c>
+      <c r="G12" s="74">
+        <v>1</v>
+      </c>
+      <c r="H12" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B13" s="77"/>
+      <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13" s="74">
+        <v>1</v>
+      </c>
+      <c r="E13" s="74">
+        <v>1</v>
+      </c>
+      <c r="F13" s="74">
+        <v>1</v>
+      </c>
+      <c r="G13" s="74">
+        <v>1</v>
+      </c>
+      <c r="H13" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="B15" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" t="s">
+        <v>193</v>
+      </c>
+      <c r="D15" s="74">
+        <v>1</v>
+      </c>
+      <c r="E15" s="74">
+        <v>1</v>
+      </c>
+      <c r="F15" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G15" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H15" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="73"/>
+      <c r="C16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D16" s="74">
+        <v>1</v>
+      </c>
+      <c r="E16" s="74">
+        <v>1</v>
+      </c>
+      <c r="F16" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G16" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H16" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B17" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="74">
+        <v>1</v>
+      </c>
+      <c r="E17" s="74">
+        <v>1</v>
+      </c>
+      <c r="F17" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G17" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H17" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B18" s="73"/>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="74">
+        <v>1</v>
+      </c>
+      <c r="E18" s="74">
+        <v>1</v>
+      </c>
+      <c r="F18" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="G18" s="74">
+        <v>1.05</v>
+      </c>
+      <c r="H18" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B19" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>193</v>
+      </c>
+      <c r="D19" s="74">
+        <v>1</v>
+      </c>
+      <c r="E19" s="74">
+        <v>1</v>
+      </c>
+      <c r="F19" s="74">
+        <v>2.5</v>
+      </c>
+      <c r="G19" s="74">
+        <v>2.5</v>
+      </c>
+      <c r="H19" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="73"/>
+      <c r="C20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D20" s="74">
+        <v>1</v>
+      </c>
+      <c r="E20" s="74">
+        <v>1</v>
+      </c>
+      <c r="F20" s="74">
+        <v>2.4</v>
+      </c>
+      <c r="G20" s="74">
+        <v>2.4</v>
+      </c>
+      <c r="H20" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="74">
+        <v>1</v>
+      </c>
+      <c r="E21" s="74">
+        <v>1</v>
+      </c>
+      <c r="F21" s="74">
+        <v>2</v>
+      </c>
+      <c r="G21" s="74">
+        <v>2</v>
+      </c>
+      <c r="H21" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="73"/>
+      <c r="C22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="74">
+        <v>1</v>
+      </c>
+      <c r="E22" s="74">
+        <v>1</v>
+      </c>
+      <c r="F22" s="74">
+        <v>1.9</v>
+      </c>
+      <c r="G22" s="74">
+        <v>1.9</v>
+      </c>
+      <c r="H22" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="74">
+        <v>1</v>
+      </c>
+      <c r="E23" s="74">
+        <v>1</v>
+      </c>
+      <c r="F23" s="74">
+        <v>1</v>
+      </c>
+      <c r="G23" s="74">
+        <v>2</v>
+      </c>
+      <c r="H23" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="73"/>
+      <c r="C24" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="74">
+        <v>1</v>
+      </c>
+      <c r="E24" s="74">
+        <v>1</v>
+      </c>
+      <c r="F24" s="74">
+        <v>1</v>
+      </c>
+      <c r="G24" s="74">
+        <v>1.9</v>
+      </c>
+      <c r="H24" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B25" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>193</v>
+      </c>
+      <c r="D25" s="74">
+        <v>1</v>
+      </c>
+      <c r="E25" s="74">
+        <v>1</v>
+      </c>
+      <c r="F25" s="74">
+        <v>1</v>
+      </c>
+      <c r="G25" s="74">
+        <v>1</v>
+      </c>
+      <c r="H25" s="74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B26" s="77"/>
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="74">
+        <v>1</v>
+      </c>
+      <c r="E26" s="74">
+        <v>1</v>
+      </c>
+      <c r="F26" s="74">
+        <v>1</v>
+      </c>
+      <c r="G26" s="74">
+        <v>1</v>
+      </c>
+      <c r="H26" s="74">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFF0000"/>
@@ -6828,7 +7713,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6889,12 +7774,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6942,7 +7827,7 @@
       <c r="A2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="78" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="3">
@@ -7021,7 +7906,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="78" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="3">
@@ -8064,7 +8949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -8298,7 +9183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -9754,7 +10639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -9845,7 +10730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFF00"/>
@@ -10493,11 +11378,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
@@ -13437,7 +14322,7 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -15366,8 +16251,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Highlights as reminder to remove data
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -58,6 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -66,6 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This is calculated, this is why it is grey -f formula should be in the input sheet</t>
@@ -80,6 +82,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -88,6 +91,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction food insecure in the target population (here the lowest 2 wealth quintiles)</t>
@@ -102,6 +106,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -110,6 +115,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 per 100,000 live births</t>
@@ -124,6 +130,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -132,6 +139,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction of pregnancies ending in spontaneous abortion</t>
@@ -146,6 +154,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -154,6 +163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Number of stillbirths per 1000 TOTAL births</t>
@@ -168,6 +178,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -176,6 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Per 1000 live births</t>
@@ -190,6 +202,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -198,6 +211,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Per 1000 live births</t>
@@ -212,6 +226,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -220,6 +235,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Per 1000 live births</t>
@@ -234,6 +250,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -242,6 +259,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Guesses</t>
@@ -256,6 +274,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -264,6 +283,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Should add up to 1</t>
@@ -278,6 +298,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -286,6 +307,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Should add up to 1</t>
@@ -311,6 +333,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -319,6 +342,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Poor pregnant women - all target population</t>
@@ -333,6 +357,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -341,6 +366,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % at risk from malaria</t>
@@ -355,6 +381,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -363,6 +390,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % at risk from malaria</t>
@@ -377,6 +405,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -385,6 +414,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % at risk from malaria</t>
@@ -399,6 +429,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -407,6 +438,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 % at risk from malaria</t>
@@ -433,6 +465,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -441,6 +474,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
@@ -455,6 +489,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -465,6 +500,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -479,6 +515,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -489,6 +526,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -503,6 +541,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -513,6 +552,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -527,6 +567,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -537,6 +578,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -551,6 +593,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -559,6 +602,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
@@ -573,6 +617,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -583,6 +628,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -597,6 +643,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -607,6 +654,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -621,6 +669,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -631,6 +680,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -645,6 +695,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -655,6 +706,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -669,6 +721,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -679,6 +732,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -693,6 +747,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -703,6 +758,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -717,6 +773,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -727,6 +784,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -741,6 +799,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -751,6 +810,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -765,6 +825,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -775,6 +836,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -789,6 +851,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -799,6 +862,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -813,6 +877,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -823,6 +888,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -837,6 +903,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User: 
 This RR is from the book.
@@ -847,6 +914,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -861,6 +929,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -869,6 +938,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Source: WHO guidelines on sprinkles</t>
@@ -883,6 +953,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -891,6 +962,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Effect on iron-deficiency anemia</t>
@@ -905,6 +977,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -913,6 +986,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Only in malaria risk</t>
@@ -927,6 +1001,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -935,6 +1010,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 made this number up
@@ -950,6 +1026,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -958,6 +1035,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Same effect as iron fortification</t>
@@ -983,6 +1061,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -991,6 +1070,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 WHO statement</t>
@@ -1005,6 +1085,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -1013,6 +1094,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST</t>
@@ -1027,6 +1109,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -1035,6 +1118,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST</t>
@@ -1062,6 +1146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -1070,6 +1155,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 made up
@@ -1085,6 +1171,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1093,6 +1180,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Horton CCC 2008: $0.9 -&gt; use $1 because of inflation</t>
@@ -1107,6 +1195,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1115,6 +1204,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 o data in the book, made up as = to IFAS for non-pregnant in hospital</t>
@@ -1129,6 +1219,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1137,6 +1228,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
@@ -1151,6 +1243,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -1159,6 +1252,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fictional</t>
@@ -1173,6 +1267,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1181,6 +1276,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Also brestfeeding women up to 6 months?</t>
@@ -1195,6 +1291,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1203,6 +1300,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 There is no unit cost for this to impact the budget.</t>
@@ -1217,6 +1315,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1225,6 +1324,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Government subsidy</t>
@@ -1239,6 +1339,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1247,6 +1348,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 There is no unit cost for this to impact the budget.</t>
@@ -1261,6 +1363,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1269,6 +1372,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Government subsidy</t>
@@ -1283,6 +1387,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -1291,6 +1396,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This is the fraction of the population eating these staples and belongs here.</t>
@@ -1305,6 +1411,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1313,6 +1420,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 orton Copenhagen Consensus 2008</t>
@@ -1327,6 +1435,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1335,6 +1444,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Same effect as iron fortification</t>
@@ -1349,6 +1459,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1357,6 +1468,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 orton Copenhagen Consensus 2008</t>
@@ -1371,6 +1483,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1379,6 +1492,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 orton Copenhagen Consensus 2008</t>
@@ -1393,6 +1507,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -1401,6 +1516,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This is the fraction of the population eating these staples and belongs here.</t>
@@ -1415,6 +1531,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1423,6 +1540,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 orton Copenhagen Consensus 2008</t>
@@ -1437,6 +1555,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -1445,6 +1564,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fictional</t>
@@ -1459,6 +1579,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -1467,6 +1588,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 From Nick</t>
@@ -1481,6 +1603,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1489,6 +1612,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Per person per year</t>
@@ -1503,6 +1627,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Microsoft Office User:</t>
         </r>
@@ -1511,6 +1636,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Made up, a bit less per treatment than PPCF per year</t>
@@ -1535,6 +1661,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1543,6 +1670,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 calculated</t>
@@ -1557,6 +1685,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1565,6 +1694,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 calculated</t>
@@ -1579,6 +1709,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1587,6 +1718,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 calculated</t>
@@ -1611,6 +1743,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -1619,6 +1752,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 From Jakub's book, annual incidence of severe acute wasting is annual prevalence * 1.6  (p. 147). Assuming the same to be true for moderate wasting.</t>
@@ -1643,6 +1777,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1651,6 +1786,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -1665,6 +1801,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1673,6 +1810,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 no data for 2 lowest age groups</t>
@@ -1687,6 +1825,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1695,6 +1834,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 no data for 2 lowest age groups</t>
@@ -1709,6 +1849,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1717,6 +1858,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 WHO database from 2001; hemoglobin &lt;110 g/L, includes mild (all-cause anemia). Consistent with Khan 2016 70.8% anemia in 6-23 months and Stevens overall ~51%</t>
@@ -1731,6 +1873,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1739,6 +1882,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 WHO database from 2001</t>
@@ -1753,6 +1897,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1761,6 +1906,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Khan 2016</t>
@@ -1775,6 +1921,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1783,6 +1930,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST - &lt;120 g/L, includes mild</t>
@@ -1797,6 +1945,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1805,6 +1954,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST &lt; 110 g/L, includes mild</t>
@@ -1819,6 +1969,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1827,6 +1978,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Default should be ~50%</t>
@@ -1841,6 +1993,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1849,6 +2002,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Stevens: 42% of global childhood anemia is ID</t>
@@ -1863,6 +2017,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1871,6 +2026,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST, includes mild</t>
@@ -1885,6 +2041,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1893,6 +2050,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST, includes mild</t>
@@ -1907,6 +2065,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1915,6 +2074,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Stevens</t>
@@ -1929,6 +2089,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1937,6 +2098,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Stevens, LiST has different values from the same source (?)</t>
@@ -1951,6 +2113,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -1959,6 +2122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Stevens; WHO definition of &lt;70g/L, LiST is has different numbers but the same source</t>
@@ -2006,6 +2170,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2014,6 +2179,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Term AGA should be given by a formula in the spreadsheet. The result should be greyed to indicate that it is calculated.</t>
@@ -2028,6 +2194,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2036,6 +2203,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Kozuki 2012, for hematocrit &lt;90g/L</t>
@@ -2062,6 +2230,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -2070,6 +2239,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LiST: 1.11</t>
@@ -2084,6 +2254,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2092,6 +2263,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This should be changed later I guess</t>
@@ -2106,6 +2278,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2114,6 +2287,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This should be changed later I guess</t>
@@ -2128,6 +2302,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -2136,6 +2311,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fictional</t>
@@ -2160,6 +2336,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -2168,6 +2345,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 May not need this listed</t>
@@ -2182,6 +2360,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -2190,6 +2369,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 We currently do not have 'appropriate complementary feeding' data to use</t>
@@ -2204,6 +2384,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Sam:</t>
         </r>
@@ -2212,6 +2393,7 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 May not need this group</t>
@@ -2238,6 +2420,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -2246,6 +2429,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
@@ -2260,6 +2444,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -2268,6 +2453,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 poor, not in malaria area
@@ -2283,6 +2469,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -2291,6 +2478,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 poor, in malaria area
@@ -2306,6 +2494,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -2314,6 +2503,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 poor, not in malaria area</t>
@@ -2328,6 +2518,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Ruth:</t>
         </r>
@@ -2336,6 +2527,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 poor, in malaria area</t>
@@ -2350,6 +2542,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -2358,6 +2551,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
@@ -2372,6 +2566,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2380,6 +2575,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
@@ -2394,6 +2590,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2402,6 +2599,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Also brestfeeding women up to 6 months?</t>
@@ -2416,6 +2614,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2424,6 +2623,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Coverage of these interventions is mutually exclusive</t>
@@ -2438,6 +2638,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2446,6 +2647,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 In baseline year, assuming only non-pregnant go to school</t>
@@ -2460,6 +2662,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -2468,6 +2671,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
@@ -2482,6 +2686,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2490,6 +2695,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 In baseline year, assuming only non-pregnant go to school</t>
@@ -2504,6 +2710,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Janka Petravic:</t>
         </r>
@@ -2512,6 +2719,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 food insecure - default poor</t>
@@ -2526,6 +2734,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2534,6 +2743,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -2548,6 +2758,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2556,6 +2767,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -2570,6 +2782,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2578,6 +2791,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -2592,6 +2806,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2600,6 +2815,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -2614,6 +2830,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2622,6 +2839,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -2636,6 +2854,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2644,6 +2863,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -2658,6 +2878,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2666,6 +2887,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -2680,6 +2902,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2688,6 +2911,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -2702,6 +2926,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2710,6 +2935,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -2724,6 +2950,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2732,6 +2959,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -2746,6 +2974,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2754,6 +2983,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -2768,6 +2998,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2776,6 +3007,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -2790,6 +3022,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2798,6 +3031,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -2812,6 +3046,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2820,6 +3055,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -2834,6 +3070,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2842,6 +3079,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -2856,6 +3094,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2864,6 +3103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2878,6 +3118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2886,6 +3127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2900,6 +3142,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2908,6 +3151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2922,6 +3166,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2930,6 +3175,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2944,6 +3190,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2952,6 +3199,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2966,6 +3214,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2974,6 +3223,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -2988,6 +3238,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -2996,6 +3247,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 At risk from malaria</t>
@@ -3010,6 +3262,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3018,6 +3271,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -3032,6 +3286,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3040,6 +3295,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -3054,6 +3310,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3062,6 +3319,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -3076,6 +3334,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3084,6 +3343,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -3098,6 +3358,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3106,6 +3367,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating wheat</t>
@@ -3120,6 +3382,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3128,6 +3391,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -3142,6 +3406,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3150,6 +3415,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -3164,6 +3430,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3172,6 +3439,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -3186,6 +3454,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3194,6 +3463,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -3208,6 +3478,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3216,6 +3487,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Fraction eating maize</t>
@@ -3230,6 +3502,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3238,6 +3511,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -3252,6 +3526,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3260,6 +3535,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -3274,6 +3550,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3282,6 +3559,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -3296,6 +3574,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3304,6 +3583,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -3318,6 +3598,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Janka Petravic:</t>
         </r>
@@ -3326,6 +3607,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 fraction eating rice</t>
@@ -4000,73 +4282,87 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -4709,7 +5005,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4827,16 +5123,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="551">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -6965,7 +7263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+    <sheetView zoomScale="111" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -6998,7 +7296,7 @@
       <c r="G1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="74" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7006,267 +7304,267 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="77" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>193</v>
       </c>
-      <c r="D2" s="74">
+      <c r="D2" s="73">
         <v>1.85</v>
       </c>
-      <c r="E2" s="74">
+      <c r="E2" s="73">
         <v>1.2</v>
       </c>
-      <c r="F2" s="74">
+      <c r="F2" s="73">
         <v>1.05</v>
       </c>
-      <c r="G2" s="74">
+      <c r="G2" s="73">
         <v>1.01</v>
       </c>
-      <c r="H2" s="76">
+      <c r="H2" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="73"/>
+      <c r="B3" s="77"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="74">
+      <c r="D3" s="73">
         <v>1.9</v>
       </c>
-      <c r="E3" s="74">
+      <c r="E3" s="73">
         <v>1.25</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="73">
         <v>1.05</v>
       </c>
-      <c r="G3" s="74">
+      <c r="G3" s="73">
         <v>1.01</v>
       </c>
-      <c r="H3" s="76">
-        <v>1</v>
-      </c>
-      <c r="J3" s="74"/>
+      <c r="H3" s="75">
+        <v>1</v>
+      </c>
+      <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="73">
         <v>2.0299999999999998</v>
       </c>
-      <c r="E4" s="74">
+      <c r="E4" s="73">
         <v>3.07</v>
       </c>
-      <c r="F4" s="74">
+      <c r="F4" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G4" s="74">
+      <c r="G4" s="73">
         <v>1.05</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="73"/>
+      <c r="B5" s="77"/>
       <c r="C5" t="s">
         <v>194</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="73">
         <v>2.17</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="73">
         <v>2.48</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G5" s="74">
+      <c r="G5" s="73">
         <v>1.05</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="74">
-        <v>1</v>
-      </c>
-      <c r="E6" s="74">
+      <c r="D6" s="73">
+        <v>1</v>
+      </c>
+      <c r="E6" s="73">
         <v>1.5</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="73">
         <v>1.3</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="73"/>
+      <c r="B7" s="77"/>
       <c r="C7" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="74">
-        <v>1</v>
-      </c>
-      <c r="E7" s="74">
+      <c r="D7" s="73">
+        <v>1</v>
+      </c>
+      <c r="E7" s="73">
         <v>1.5</v>
       </c>
-      <c r="F7" s="74">
+      <c r="F7" s="73">
         <v>1.25</v>
       </c>
-      <c r="G7" s="74">
+      <c r="G7" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H7" s="76">
+      <c r="H7" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="77" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>193</v>
       </c>
-      <c r="D8" s="74">
-        <v>1</v>
-      </c>
-      <c r="E8" s="74">
-        <v>1</v>
-      </c>
-      <c r="F8" s="74">
+      <c r="D8" s="73">
+        <v>1</v>
+      </c>
+      <c r="E8" s="73">
+        <v>1</v>
+      </c>
+      <c r="F8" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="73"/>
+      <c r="B9" s="77"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
-      <c r="D9" s="74">
-        <v>1</v>
-      </c>
-      <c r="E9" s="74">
-        <v>1</v>
-      </c>
-      <c r="F9" s="74">
+      <c r="D9" s="73">
+        <v>1</v>
+      </c>
+      <c r="E9" s="73">
+        <v>1</v>
+      </c>
+      <c r="F9" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="G9" s="74">
+      <c r="G9" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H9" s="76">
+      <c r="H9" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="77" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>193</v>
       </c>
-      <c r="D10" s="74">
-        <v>1</v>
-      </c>
-      <c r="E10" s="74">
-        <v>1</v>
-      </c>
-      <c r="F10" s="74">
-        <v>1</v>
-      </c>
-      <c r="G10" s="74">
+      <c r="D10" s="73">
+        <v>1</v>
+      </c>
+      <c r="E10" s="73">
+        <v>1</v>
+      </c>
+      <c r="F10" s="73">
+        <v>1</v>
+      </c>
+      <c r="G10" s="73">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H10" s="76">
+      <c r="H10" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="73"/>
+      <c r="B11" s="77"/>
       <c r="C11" t="s">
         <v>194</v>
       </c>
-      <c r="D11" s="74">
-        <v>1</v>
-      </c>
-      <c r="E11" s="74">
-        <v>1</v>
-      </c>
-      <c r="F11" s="74">
-        <v>1</v>
-      </c>
-      <c r="G11" s="74">
+      <c r="D11" s="73">
+        <v>1</v>
+      </c>
+      <c r="E11" s="73">
+        <v>1</v>
+      </c>
+      <c r="F11" s="73">
+        <v>1</v>
+      </c>
+      <c r="G11" s="73">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H11" s="76">
+      <c r="H11" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="78" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
         <v>193</v>
       </c>
-      <c r="D12" s="74">
-        <v>1</v>
-      </c>
-      <c r="E12" s="74">
-        <v>1</v>
-      </c>
-      <c r="F12" s="74">
-        <v>1</v>
-      </c>
-      <c r="G12" s="74">
-        <v>1</v>
-      </c>
-      <c r="H12" s="76">
+      <c r="D12" s="73">
+        <v>1</v>
+      </c>
+      <c r="E12" s="73">
+        <v>1</v>
+      </c>
+      <c r="F12" s="73">
+        <v>1</v>
+      </c>
+      <c r="G12" s="73">
+        <v>1</v>
+      </c>
+      <c r="H12" s="75">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="77"/>
+      <c r="B13" s="78"/>
       <c r="C13" t="s">
         <v>194</v>
       </c>
-      <c r="D13" s="74">
-        <v>1</v>
-      </c>
-      <c r="E13" s="74">
-        <v>1</v>
-      </c>
-      <c r="F13" s="74">
-        <v>1</v>
-      </c>
-      <c r="G13" s="74">
-        <v>1</v>
-      </c>
-      <c r="H13" s="76">
+      <c r="D13" s="73">
+        <v>1</v>
+      </c>
+      <c r="E13" s="73">
+        <v>1</v>
+      </c>
+      <c r="F13" s="73">
+        <v>1</v>
+      </c>
+      <c r="G13" s="73">
+        <v>1</v>
+      </c>
+      <c r="H13" s="75">
         <v>1</v>
       </c>
     </row>
@@ -7274,276 +7572,271 @@
       <c r="A15" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="77" t="s">
         <v>81</v>
       </c>
       <c r="C15" t="s">
         <v>193</v>
       </c>
-      <c r="D15" s="74">
-        <v>1</v>
-      </c>
-      <c r="E15" s="74">
-        <v>1</v>
-      </c>
-      <c r="F15" s="74">
+      <c r="D15" s="73">
+        <v>1</v>
+      </c>
+      <c r="E15" s="73">
+        <v>1</v>
+      </c>
+      <c r="F15" s="73">
         <v>1.05</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="73">
         <v>1.05</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="73"/>
+      <c r="B16" s="77"/>
       <c r="C16" t="s">
         <v>194</v>
       </c>
-      <c r="D16" s="74">
-        <v>1</v>
-      </c>
-      <c r="E16" s="74">
-        <v>1</v>
-      </c>
-      <c r="F16" s="74">
+      <c r="D16" s="73">
+        <v>1</v>
+      </c>
+      <c r="E16" s="73">
+        <v>1</v>
+      </c>
+      <c r="F16" s="73">
         <v>1.05</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="73">
         <v>1.05</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H16" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="73" t="s">
+      <c r="B17" s="77" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
         <v>193</v>
       </c>
-      <c r="D17" s="74">
-        <v>1</v>
-      </c>
-      <c r="E17" s="74">
-        <v>1</v>
-      </c>
-      <c r="F17" s="74">
+      <c r="D17" s="73">
+        <v>1</v>
+      </c>
+      <c r="E17" s="73">
+        <v>1</v>
+      </c>
+      <c r="F17" s="73">
         <v>1.05</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="73">
         <v>1.05</v>
       </c>
-      <c r="H17" s="74">
+      <c r="H17" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="73"/>
+      <c r="B18" s="77"/>
       <c r="C18" t="s">
         <v>194</v>
       </c>
-      <c r="D18" s="74">
-        <v>1</v>
-      </c>
-      <c r="E18" s="74">
-        <v>1</v>
-      </c>
-      <c r="F18" s="74">
+      <c r="D18" s="73">
+        <v>1</v>
+      </c>
+      <c r="E18" s="73">
+        <v>1</v>
+      </c>
+      <c r="F18" s="73">
         <v>1.05</v>
       </c>
-      <c r="G18" s="74">
+      <c r="G18" s="73">
         <v>1.05</v>
       </c>
-      <c r="H18" s="74">
+      <c r="H18" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="73" t="s">
+      <c r="B19" s="77" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
         <v>193</v>
       </c>
-      <c r="D19" s="74">
-        <v>1</v>
-      </c>
-      <c r="E19" s="74">
-        <v>1</v>
-      </c>
-      <c r="F19" s="74">
+      <c r="D19" s="73">
+        <v>1</v>
+      </c>
+      <c r="E19" s="73">
+        <v>1</v>
+      </c>
+      <c r="F19" s="73">
         <v>2.5</v>
       </c>
-      <c r="G19" s="74">
+      <c r="G19" s="73">
         <v>2.5</v>
       </c>
-      <c r="H19" s="74">
+      <c r="H19" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="73"/>
+      <c r="B20" s="77"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
-      <c r="D20" s="74">
-        <v>1</v>
-      </c>
-      <c r="E20" s="74">
-        <v>1</v>
-      </c>
-      <c r="F20" s="74">
+      <c r="D20" s="73">
+        <v>1</v>
+      </c>
+      <c r="E20" s="73">
+        <v>1</v>
+      </c>
+      <c r="F20" s="73">
         <v>2.4</v>
       </c>
-      <c r="G20" s="74">
+      <c r="G20" s="73">
         <v>2.4</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H20" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="77" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
         <v>193</v>
       </c>
-      <c r="D21" s="74">
-        <v>1</v>
-      </c>
-      <c r="E21" s="74">
-        <v>1</v>
-      </c>
-      <c r="F21" s="74">
+      <c r="D21" s="73">
+        <v>1</v>
+      </c>
+      <c r="E21" s="73">
+        <v>1</v>
+      </c>
+      <c r="F21" s="73">
         <v>2</v>
       </c>
-      <c r="G21" s="74">
+      <c r="G21" s="73">
         <v>2</v>
       </c>
-      <c r="H21" s="74">
+      <c r="H21" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="73"/>
+      <c r="B22" s="77"/>
       <c r="C22" t="s">
         <v>194</v>
       </c>
-      <c r="D22" s="74">
-        <v>1</v>
-      </c>
-      <c r="E22" s="74">
-        <v>1</v>
-      </c>
-      <c r="F22" s="74">
+      <c r="D22" s="73">
+        <v>1</v>
+      </c>
+      <c r="E22" s="73">
+        <v>1</v>
+      </c>
+      <c r="F22" s="73">
         <v>1.9</v>
       </c>
-      <c r="G22" s="74">
+      <c r="G22" s="73">
         <v>1.9</v>
       </c>
-      <c r="H22" s="74">
+      <c r="H22" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="73" t="s">
+      <c r="B23" s="77" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
         <v>193</v>
       </c>
-      <c r="D23" s="74">
-        <v>1</v>
-      </c>
-      <c r="E23" s="74">
-        <v>1</v>
-      </c>
-      <c r="F23" s="74">
-        <v>1</v>
-      </c>
-      <c r="G23" s="74">
+      <c r="D23" s="73">
+        <v>1</v>
+      </c>
+      <c r="E23" s="73">
+        <v>1</v>
+      </c>
+      <c r="F23" s="73">
+        <v>1</v>
+      </c>
+      <c r="G23" s="73">
         <v>2</v>
       </c>
-      <c r="H23" s="74">
+      <c r="H23" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="73"/>
+      <c r="B24" s="77"/>
       <c r="C24" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="74">
-        <v>1</v>
-      </c>
-      <c r="E24" s="74">
-        <v>1</v>
-      </c>
-      <c r="F24" s="74">
-        <v>1</v>
-      </c>
-      <c r="G24" s="74">
+      <c r="D24" s="73">
+        <v>1</v>
+      </c>
+      <c r="E24" s="73">
+        <v>1</v>
+      </c>
+      <c r="F24" s="73">
+        <v>1</v>
+      </c>
+      <c r="G24" s="73">
         <v>1.9</v>
       </c>
-      <c r="H24" s="74">
+      <c r="H24" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="78" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
         <v>193</v>
       </c>
-      <c r="D25" s="74">
-        <v>1</v>
-      </c>
-      <c r="E25" s="74">
-        <v>1</v>
-      </c>
-      <c r="F25" s="74">
-        <v>1</v>
-      </c>
-      <c r="G25" s="74">
-        <v>1</v>
-      </c>
-      <c r="H25" s="74">
+      <c r="D25" s="73">
+        <v>1</v>
+      </c>
+      <c r="E25" s="73">
+        <v>1</v>
+      </c>
+      <c r="F25" s="73">
+        <v>1</v>
+      </c>
+      <c r="G25" s="73">
+        <v>1</v>
+      </c>
+      <c r="H25" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="77"/>
+      <c r="B26" s="78"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
-      <c r="D26" s="74">
-        <v>1</v>
-      </c>
-      <c r="E26" s="74">
-        <v>1</v>
-      </c>
-      <c r="F26" s="74">
-        <v>1</v>
-      </c>
-      <c r="G26" s="74">
-        <v>1</v>
-      </c>
-      <c r="H26" s="74">
+      <c r="D26" s="73">
+        <v>1</v>
+      </c>
+      <c r="E26" s="73">
+        <v>1</v>
+      </c>
+      <c r="F26" s="73">
+        <v>1</v>
+      </c>
+      <c r="G26" s="73">
+        <v>1</v>
+      </c>
+      <c r="H26" s="73">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
@@ -7551,6 +7844,11 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7779,7 +8077,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7827,7 +8125,7 @@
       <c r="A2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="76" t="s">
         <v>56</v>
       </c>
       <c r="C2" s="3">
@@ -7906,7 +8204,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="76" t="s">
         <v>57</v>
       </c>
       <c r="C5" s="3">
@@ -16251,8 +16549,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -16453,10 +16751,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="76" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="6">
@@ -16476,7 +16774,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="80"/>
+      <c r="B13" s="76" t="s">
         <v>57</v>
       </c>
       <c r="C13" s="6">

</xml_diff>

<commit_message>
Unchecked boxes for IYCF programs
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3619,7 +3619,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -4234,9 +4234,6 @@
   </si>
   <si>
     <t>Mass media</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -5127,14 +5124,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="551">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7304,7 +7301,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="80" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -7327,7 +7324,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="77"/>
+      <c r="B3" s="80"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -7349,7 +7346,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -7372,7 +7369,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="77"/>
+      <c r="B5" s="80"/>
       <c r="C5" t="s">
         <v>194</v>
       </c>
@@ -7393,7 +7390,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="80" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -7416,7 +7413,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="77"/>
+      <c r="B7" s="80"/>
       <c r="C7" t="s">
         <v>194</v>
       </c>
@@ -7437,7 +7434,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="80" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
@@ -7460,7 +7457,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="77"/>
+      <c r="B9" s="80"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -7481,7 +7478,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="80" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -7504,7 +7501,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="77"/>
+      <c r="B11" s="80"/>
       <c r="C11" t="s">
         <v>194</v>
       </c>
@@ -7525,7 +7522,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="79" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
@@ -7548,7 +7545,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="78"/>
+      <c r="B13" s="79"/>
       <c r="C13" t="s">
         <v>194</v>
       </c>
@@ -7572,7 +7569,7 @@
       <c r="A15" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="80" t="s">
         <v>81</v>
       </c>
       <c r="C15" t="s">
@@ -7595,7 +7592,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="77"/>
+      <c r="B16" s="80"/>
       <c r="C16" t="s">
         <v>194</v>
       </c>
@@ -7616,7 +7613,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="80" t="s">
         <v>6</v>
       </c>
       <c r="C17" t="s">
@@ -7639,7 +7636,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="77"/>
+      <c r="B18" s="80"/>
       <c r="C18" t="s">
         <v>194</v>
       </c>
@@ -7660,7 +7657,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="80" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
@@ -7683,7 +7680,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="77"/>
+      <c r="B20" s="80"/>
       <c r="C20" t="s">
         <v>194</v>
       </c>
@@ -7704,7 +7701,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="77" t="s">
+      <c r="B21" s="80" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
@@ -7727,7 +7724,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="77"/>
+      <c r="B22" s="80"/>
       <c r="C22" t="s">
         <v>194</v>
       </c>
@@ -7748,7 +7745,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="80" t="s">
         <v>9</v>
       </c>
       <c r="C23" t="s">
@@ -7771,7 +7768,7 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="77"/>
+      <c r="B24" s="80"/>
       <c r="C24" t="s">
         <v>194</v>
       </c>
@@ -7792,7 +7789,7 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="78" t="s">
+      <c r="B25" s="79" t="s">
         <v>10</v>
       </c>
       <c r="C25" t="s">
@@ -7815,7 +7812,7 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="78"/>
+      <c r="B26" s="79"/>
       <c r="C26" t="s">
         <v>194</v>
       </c>
@@ -7859,8 +7856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7894,41 +7891,26 @@
       <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
@@ -7937,25 +7919,16 @@
       <c r="B8" t="s">
         <v>81</v>
       </c>
-      <c r="D8" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
@@ -7965,9 +7938,6 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -16549,7 +16519,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -16751,7 +16721,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="79" t="s">
+      <c r="A12" s="77" t="s">
         <v>122</v>
       </c>
       <c r="B12" s="76" t="s">
@@ -16774,7 +16744,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="76" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
Added in mass media impact for IYCF
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="-35860" yWindow="-20720" windowWidth="28520" windowHeight="20720" tabRatio="500" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -321,11 +321,12 @@
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>Janka Petravic</author>
+    <author>Ruth</author>
     <author xml:space="preserve"> Janka Petravic</author>
-    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="E6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -335,7 +336,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
+          <t>Janka Petravic:</t>
         </r>
         <r>
           <rPr>
@@ -345,103 +346,1185 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Poor pregnant women - all target population</t>
+food insecure - default poor</t>
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="1">
+    <comment ref="E7" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, not in malaria area
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="1">
+    <comment ref="E8" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, in malaria area
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="1">
+    <comment ref="E9" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, not in malaria area</t>
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="1">
+    <comment ref="E10" authorId="1">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-% at risk from malaria</t>
+poor, in malaria area</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Also brestfeeding women up to 6 months?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Coverage of these interventions is mutually exclusive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I22" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I29" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+In baseline year, assuming only non-pregnant go to school</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+food insecure - default poor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I37" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I38" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I39" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I41" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+At risk from malaria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I42" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating wheat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I43" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fraction eating maize</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I44" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+fraction eating rice</t>
         </r>
       </text>
     </comment>
@@ -454,10 +1537,9 @@
   <authors>
     <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -477,11 +1559,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+Poor pregnant women - all target population</t>
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="1">
+    <comment ref="C9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -491,9 +1573,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -503,11 +1583,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="1">
+    <comment ref="D9" authorId="1">
       <text>
         <r>
           <rPr>
@@ -517,9 +1597,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -529,11 +1607,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="N2" authorId="1">
+    <comment ref="C11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -543,9 +1621,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -555,11 +1631,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
-    <comment ref="O2" authorId="1">
+    <comment ref="D11" authorId="1">
       <text>
         <r>
           <rPr>
@@ -569,9 +1645,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+          <t>Microsoft Office User:</t>
         </r>
         <r>
           <rPr>
@@ -581,464 +1655,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O3" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O4" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O5" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User: 
-This RR is from the book.
-LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Source: WHO guidelines on sprinkles</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E23" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Effect on iron-deficiency anemia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Only in malaria risk</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E30" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-made this number up
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B31" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Same effect as iron fortification</t>
+% at risk from malaria</t>
         </r>
       </text>
     </comment>
@@ -1049,11 +1666,36 @@
 <file path=xl/comments12.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author xml:space="preserve"> Janka Petravic</author>
     <author>Microsoft Office User</author>
-    <author>Sam</author>
+    <author>Ruth</author>
   </authors>
   <commentList>
-    <comment ref="F21" authorId="0">
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1063,7 +1705,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Microsoft Office User:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1073,11 +1717,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-WHO statement</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="1">
+    <comment ref="M2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1087,7 +1731,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1097,11 +1743,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="D23" authorId="1">
+    <comment ref="N2" authorId="1">
       <text>
         <r>
           <rPr>
@@ -1111,7 +1757,9 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>Sam:</t>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
         </r>
         <r>
           <rPr>
@@ -1121,7 +1769,490 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-LiST</t>
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> Janka Petravic:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O3" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O4" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User: 
+This RR is from the book.
+LiST uses RR=0.63 for all-cause ; RR=0.33  for IDA</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Source: WHO guidelines on sprinkles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Effect on iron-deficiency anemia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Only in malaria risk</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E30" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Ruth:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+made this number up
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Same effect as iron fortification</t>
         </r>
       </text>
     </comment>
@@ -1130,6 +2261,89 @@
 </file>
 
 <file path=xl/comments13.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="F21" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+WHO statement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D23" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+LiST</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments14.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Ruth</author>
@@ -2328,7 +3542,7 @@
     <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2348,55 +3562,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-May not need this listed</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-We currently do not have 'appropriate complementary feeding' data to use</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-May not need this group</t>
+We currently do not have 'appropriate complementary feeding' data to use, so this does nothing.</t>
         </r>
       </text>
     </comment>
@@ -2407,1210 +3573,49 @@
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Janka Petravic</author>
-    <author>Ruth</author>
-    <author xml:space="preserve"> Janka Petravic</author>
+    <author>Sam</author>
   </authors>
   <commentList>
-    <comment ref="E6" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="1">
-      <text>
+If user wants this, it must be checked for </t>
+        </r>
         <r>
           <rPr>
             <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, not in malaria area
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, in malaria area
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, not in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E10" authorId="1">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Ruth:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-poor, in malaria area</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H15" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Mutually exclusive with AMS, target = 1 - coverage of AMS - pregnant at risk of malaria not receiving IPTp or bednets</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B20" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Also brestfeeding women up to 6 months?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A22" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Coverage of these interventions is mutually exclusive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I22" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I29" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-In baseline year, assuming only non-pregnant go to school</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I30" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-food insecure - default poor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I37" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I38" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I39" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I41" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-At risk from malaria</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I42" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating wheat</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I43" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Fraction eating maize</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I44" authorId="2">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> Janka Petravic:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-fraction eating rice</t>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>all populations</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> b/c they are all targetted at once.</t>
         </r>
       </text>
     </comment>
@@ -3619,7 +3624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="206">
   <si>
     <t>year</t>
   </si>
@@ -4234,6 +4239,9 @@
   </si>
   <si>
     <t>Mass media</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -4362,7 +4370,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4411,6 +4419,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -5002,7 +5016,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5126,12 +5140,17 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="551">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7258,10 +7277,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7523,57 +7542,64 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B12" s="79" t="s">
-        <v>10</v>
+        <v>112</v>
       </c>
       <c r="C12" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="E12" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="F12" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="G12" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="H12" s="82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="77" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
         <v>193</v>
       </c>
-      <c r="D12" s="73">
-        <v>1</v>
-      </c>
-      <c r="E12" s="73">
-        <v>1</v>
-      </c>
-      <c r="F12" s="73">
-        <v>1</v>
-      </c>
-      <c r="G12" s="73">
-        <v>1</v>
-      </c>
-      <c r="H12" s="75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B13" s="79"/>
-      <c r="C13" t="s">
+      <c r="D14" s="73">
+        <v>1</v>
+      </c>
+      <c r="E14" s="73">
+        <v>1</v>
+      </c>
+      <c r="F14" s="73">
+        <v>1.05</v>
+      </c>
+      <c r="G14" s="73">
+        <v>1.05</v>
+      </c>
+      <c r="H14" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="80"/>
+      <c r="C15" t="s">
         <v>194</v>
-      </c>
-      <c r="D13" s="73">
-        <v>1</v>
-      </c>
-      <c r="E13" s="73">
-        <v>1</v>
-      </c>
-      <c r="F13" s="73">
-        <v>1</v>
-      </c>
-      <c r="G13" s="73">
-        <v>1</v>
-      </c>
-      <c r="H13" s="75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A15" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="B15" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" t="s">
-        <v>193</v>
       </c>
       <c r="D15" s="73">
         <v>1</v>
@@ -7592,9 +7618,11 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="80"/>
+      <c r="B16" s="80" t="s">
+        <v>6</v>
+      </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D16" s="73">
         <v>1</v>
@@ -7613,11 +7641,9 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="80" t="s">
-        <v>6</v>
-      </c>
+      <c r="B17" s="80"/>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D17" s="73">
         <v>1</v>
@@ -7636,216 +7662,172 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="80"/>
+      <c r="B18" s="80" t="s">
+        <v>7</v>
+      </c>
       <c r="C18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D18" s="73">
+        <v>1</v>
+      </c>
+      <c r="E18" s="73">
+        <v>1</v>
+      </c>
+      <c r="F18" s="73">
+        <v>2.5</v>
+      </c>
+      <c r="G18" s="73">
+        <v>2.5</v>
+      </c>
+      <c r="H18" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B19" s="80"/>
+      <c r="C19" t="s">
         <v>194</v>
       </c>
-      <c r="D18" s="73">
-        <v>1</v>
-      </c>
-      <c r="E18" s="73">
-        <v>1</v>
-      </c>
-      <c r="F18" s="73">
+      <c r="D19" s="73">
+        <v>1</v>
+      </c>
+      <c r="E19" s="73">
+        <v>1</v>
+      </c>
+      <c r="F19" s="73">
+        <v>2.4</v>
+      </c>
+      <c r="G19" s="73">
+        <v>2.4</v>
+      </c>
+      <c r="H19" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B20" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="73">
+        <v>1</v>
+      </c>
+      <c r="E20" s="73">
+        <v>1</v>
+      </c>
+      <c r="F20" s="73">
+        <v>2</v>
+      </c>
+      <c r="G20" s="73">
+        <v>2</v>
+      </c>
+      <c r="H20" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B21" s="80"/>
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="73">
+        <v>1</v>
+      </c>
+      <c r="E21" s="73">
+        <v>1</v>
+      </c>
+      <c r="F21" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="G21" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="H21" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B22" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="73">
+        <v>1</v>
+      </c>
+      <c r="E22" s="73">
+        <v>1</v>
+      </c>
+      <c r="F22" s="73">
+        <v>1</v>
+      </c>
+      <c r="G22" s="73">
+        <v>2</v>
+      </c>
+      <c r="H22" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B23" s="80"/>
+      <c r="C23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D23" s="73">
+        <v>1</v>
+      </c>
+      <c r="E23" s="73">
+        <v>1</v>
+      </c>
+      <c r="F23" s="73">
+        <v>1</v>
+      </c>
+      <c r="G23" s="73">
+        <v>1.9</v>
+      </c>
+      <c r="H23" s="73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+      <c r="B24" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D24" s="82">
         <v>1.05</v>
       </c>
-      <c r="G18" s="73">
+      <c r="E24" s="82">
         <v>1.05</v>
       </c>
-      <c r="H18" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>193</v>
-      </c>
-      <c r="D19" s="73">
-        <v>1</v>
-      </c>
-      <c r="E19" s="73">
-        <v>1</v>
-      </c>
-      <c r="F19" s="73">
-        <v>2.5</v>
-      </c>
-      <c r="G19" s="73">
-        <v>2.5</v>
-      </c>
-      <c r="H19" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="80"/>
-      <c r="C20" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="73">
-        <v>1</v>
-      </c>
-      <c r="E20" s="73">
-        <v>1</v>
-      </c>
-      <c r="F20" s="73">
-        <v>2.4</v>
-      </c>
-      <c r="G20" s="73">
-        <v>2.4</v>
-      </c>
-      <c r="H20" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" s="73">
-        <v>1</v>
-      </c>
-      <c r="E21" s="73">
-        <v>1</v>
-      </c>
-      <c r="F21" s="73">
-        <v>2</v>
-      </c>
-      <c r="G21" s="73">
-        <v>2</v>
-      </c>
-      <c r="H21" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="80"/>
-      <c r="C22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D22" s="73">
-        <v>1</v>
-      </c>
-      <c r="E22" s="73">
-        <v>1</v>
-      </c>
-      <c r="F22" s="73">
-        <v>1.9</v>
-      </c>
-      <c r="G22" s="73">
-        <v>1.9</v>
-      </c>
-      <c r="H22" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>193</v>
-      </c>
-      <c r="D23" s="73">
-        <v>1</v>
-      </c>
-      <c r="E23" s="73">
-        <v>1</v>
-      </c>
-      <c r="F23" s="73">
-        <v>1</v>
-      </c>
-      <c r="G23" s="73">
-        <v>2</v>
-      </c>
-      <c r="H23" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="80"/>
-      <c r="C24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D24" s="73">
-        <v>1</v>
-      </c>
-      <c r="E24" s="73">
-        <v>1</v>
-      </c>
-      <c r="F24" s="73">
-        <v>1</v>
-      </c>
-      <c r="G24" s="73">
-        <v>1.9</v>
-      </c>
-      <c r="H24" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B25" s="79" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" t="s">
-        <v>193</v>
-      </c>
-      <c r="D25" s="73">
-        <v>1</v>
-      </c>
-      <c r="E25" s="73">
-        <v>1</v>
-      </c>
-      <c r="F25" s="73">
-        <v>1</v>
-      </c>
-      <c r="G25" s="73">
-        <v>1</v>
-      </c>
-      <c r="H25" s="73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="79"/>
-      <c r="C26" t="s">
-        <v>194</v>
-      </c>
-      <c r="D26" s="73">
-        <v>1</v>
-      </c>
-      <c r="E26" s="73">
-        <v>1</v>
-      </c>
-      <c r="F26" s="73">
-        <v>1</v>
-      </c>
-      <c r="G26" s="73">
-        <v>1</v>
-      </c>
-      <c r="H26" s="73">
+      <c r="F24" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="G24" s="82">
+        <v>1.05</v>
+      </c>
+      <c r="H24" s="82">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B25:B26"/>
+  <mergeCells count="10">
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7853,11 +7835,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7891,85 +7873,128 @@
       <c r="B2" t="s">
         <v>81</v>
       </c>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" s="83"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" s="83"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="83"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="s">
+      <c r="D6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E6" s="83"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
+      <c r="E9" s="83"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E10" s="83"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E11" s="83"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="83"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B13" t="s">
         <v>9</v>
       </c>
+      <c r="E13" s="83"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="10" t="s">
+      <c r="B14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B15" t="s">
+      <c r="E16" s="83"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
+      <c r="E17" s="83"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+      <c r="E18" s="83"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
-      <c r="B18" t="s">
+      <c r="E19" s="83"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
+      <c r="E20" s="83"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="83"/>
+      <c r="D21" s="83"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates for wasting re-run CHANGE BACK (left TODOs there)
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
+++ b/input_spreadsheets/Bangladesh/2017Oct/InputForCode_Bangladesh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35860" yWindow="-20720" windowWidth="28520" windowHeight="20720" tabRatio="500" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="-35860" yWindow="-20720" windowWidth="28520" windowHeight="20720" tabRatio="500" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year demographics" sheetId="1" r:id="rId1"/>
@@ -3624,7 +3624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="205">
   <si>
     <t>year</t>
   </si>
@@ -4239,9 +4239,6 @@
   </si>
   <si>
     <t>Mass media</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
@@ -5143,14 +5140,14 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="551">
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
@@ -7320,7 +7317,7 @@
       <c r="A2" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="83" t="s">
         <v>81</v>
       </c>
       <c r="C2" t="s">
@@ -7343,7 +7340,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B3" s="80"/>
+      <c r="B3" s="83"/>
       <c r="C3" t="s">
         <v>194</v>
       </c>
@@ -7365,7 +7362,7 @@
       <c r="J3" s="73"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="83" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
@@ -7388,7 +7385,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B5" s="80"/>
+      <c r="B5" s="83"/>
       <c r="C5" t="s">
         <v>194</v>
       </c>
@@ -7409,7 +7406,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="83" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
@@ -7432,7 +7429,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B7" s="80"/>
+      <c r="B7" s="83"/>
       <c r="C7" t="s">
         <v>194</v>
       </c>
@@ -7453,7 +7450,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="83" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
@@ -7476,7 +7473,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B9" s="80"/>
+      <c r="B9" s="83"/>
       <c r="C9" t="s">
         <v>194</v>
       </c>
@@ -7497,7 +7494,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="83" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -7520,7 +7517,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B11" s="80"/>
+      <c r="B11" s="83"/>
       <c r="C11" t="s">
         <v>194</v>
       </c>
@@ -7547,19 +7544,19 @@
       <c r="C12" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="81">
         <v>1.05</v>
       </c>
-      <c r="E12" s="82">
+      <c r="E12" s="81">
         <v>1.05</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="81">
         <v>1.05</v>
       </c>
-      <c r="G12" s="82">
+      <c r="G12" s="81">
         <v>1.05</v>
       </c>
-      <c r="H12" s="82">
+      <c r="H12" s="81">
         <v>1</v>
       </c>
     </row>
@@ -7574,7 +7571,7 @@
       <c r="A14" s="77" t="s">
         <v>198</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="83" t="s">
         <v>81</v>
       </c>
       <c r="C14" t="s">
@@ -7597,7 +7594,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B15" s="80"/>
+      <c r="B15" s="83"/>
       <c r="C15" t="s">
         <v>194</v>
       </c>
@@ -7618,7 +7615,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B16" s="80" t="s">
+      <c r="B16" s="83" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
@@ -7641,7 +7638,7 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B17" s="80"/>
+      <c r="B17" s="83"/>
       <c r="C17" t="s">
         <v>194</v>
       </c>
@@ -7662,7 +7659,7 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B18" s="80" t="s">
+      <c r="B18" s="83" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
@@ -7685,7 +7682,7 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="80"/>
+      <c r="B19" s="83"/>
       <c r="C19" t="s">
         <v>194</v>
       </c>
@@ -7706,7 +7703,7 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B20" s="80" t="s">
+      <c r="B20" s="83" t="s">
         <v>8</v>
       </c>
       <c r="C20" t="s">
@@ -7729,7 +7726,7 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="80"/>
+      <c r="B21" s="83"/>
       <c r="C21" t="s">
         <v>194</v>
       </c>
@@ -7750,7 +7747,7 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="80" t="s">
+      <c r="B22" s="83" t="s">
         <v>9</v>
       </c>
       <c r="C22" t="s">
@@ -7773,7 +7770,7 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B23" s="80"/>
+      <c r="B23" s="83"/>
       <c r="C23" t="s">
         <v>194</v>
       </c>
@@ -7794,25 +7791,25 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B24" s="81" t="s">
+      <c r="B24" s="80" t="s">
         <v>112</v>
       </c>
       <c r="C24" t="s">
         <v>204</v>
       </c>
-      <c r="D24" s="82">
+      <c r="D24" s="81">
         <v>1.05</v>
       </c>
-      <c r="E24" s="82">
+      <c r="E24" s="81">
         <v>1.05</v>
       </c>
-      <c r="F24" s="82">
+      <c r="F24" s="81">
         <v>1.05</v>
       </c>
-      <c r="G24" s="82">
+      <c r="G24" s="81">
         <v>1.05</v>
       </c>
-      <c r="H24" s="82">
+      <c r="H24" s="81">
         <v>1</v>
       </c>
     </row>
@@ -7838,8 +7835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView zoomScale="133" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7873,44 +7870,38 @@
       <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="83"/>
+      <c r="E2" s="82"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="83"/>
+      <c r="E3" s="82"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="83"/>
+      <c r="E4" s="82"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="83"/>
+      <c r="E5" s="82"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E6" s="83"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>112</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="10" t="s">
@@ -7919,38 +7910,38 @@
       <c r="B9" t="s">
         <v>81</v>
       </c>
-      <c r="E9" s="83"/>
+      <c r="E9" s="82"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="83"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="83"/>
+      <c r="E11" s="82"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="83"/>
+      <c r="E12" s="82"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="83"/>
+      <c r="E13" s="82"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A16" s="10" t="s">
@@ -7959,38 +7950,38 @@
       <c r="B16" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="83"/>
+      <c r="E16" s="82"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="83"/>
+      <c r="E17" s="82"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="83"/>
+      <c r="E18" s="82"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="83"/>
+      <c r="E19" s="82"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="83"/>
+      <c r="E20" s="82"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>112</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16544,7 +16535,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>